<commit_message>
fix the idx for phone
</commit_message>
<xml_diff>
--- a/data/2018年6月份联通话单.xlsx
+++ b/data/2018年6月份联通话单.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luzhiming/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangzhen/gitRepository/csv2graph/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13460" yWindow="460" windowWidth="29620" windowHeight="18840" tabRatio="500"/>
+    <workbookView xWindow="2560" yWindow="-16760" windowWidth="28040" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -628,7 +628,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -652,12 +652,13 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -934,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,7 +1043,7 @@
       </c>
       <c r="J2" s="1" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,3),1515204,1589525,1390522)&amp;TEXT(RANDBETWEEN(0,10^4-1),"0000")</f>
-        <v>13905229034</v>
+        <v>15895254870</v>
       </c>
       <c r="K2" s="8">
         <v>43253.589918981481</v>
@@ -1099,7 +1100,7 @@
       </c>
       <c r="J3" s="1" t="str">
         <f t="shared" ref="J3:J21" ca="1" si="0">CHOOSE(RANDBETWEEN(1,3),1515204,1589525,1390522)&amp;TEXT(RANDBETWEEN(0,10^4-1),"0000")</f>
-        <v>13905229482</v>
+        <v>13905228189</v>
       </c>
       <c r="K3" s="8">
         <v>43255.567303240743</v>
@@ -1156,7 +1157,7 @@
       </c>
       <c r="J4" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13905226747</v>
+        <v>15895259763</v>
       </c>
       <c r="K4" s="8">
         <v>43255.761886574073</v>
@@ -1213,7 +1214,7 @@
       </c>
       <c r="J5" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13905226676</v>
+        <v>15895253831</v>
       </c>
       <c r="K5" s="8">
         <v>43255.815023148149</v>
@@ -1270,7 +1271,7 @@
       </c>
       <c r="J6" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895255820</v>
+        <v>13905225558</v>
       </c>
       <c r="K6" s="8">
         <v>43255.815833333334</v>
@@ -1327,7 +1328,7 @@
       </c>
       <c r="J7" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13905220035</v>
+        <v>13905221101</v>
       </c>
       <c r="K7" s="8">
         <v>43255.855127314811</v>
@@ -1384,7 +1385,7 @@
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895254413</v>
+        <v>15152043412</v>
       </c>
       <c r="K8" s="8">
         <v>43257.343472222223</v>
@@ -1441,7 +1442,7 @@
       </c>
       <c r="J9" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895255120</v>
+        <v>15152041642</v>
       </c>
       <c r="K9" s="8">
         <v>43257.729143518518</v>
@@ -1498,7 +1499,7 @@
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895259659</v>
+        <v>13905228035</v>
       </c>
       <c r="K10" s="8">
         <v>43257.775324074071</v>
@@ -1555,7 +1556,7 @@
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895252548</v>
+        <v>15895256576</v>
       </c>
       <c r="K11" s="8">
         <v>43258.491076388891</v>
@@ -1612,7 +1613,7 @@
       </c>
       <c r="J12" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13905228698</v>
+        <v>15152041691</v>
       </c>
       <c r="K12" s="8">
         <v>43258.491678240738</v>
@@ -1669,7 +1670,7 @@
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895257601</v>
+        <v>15152047166</v>
       </c>
       <c r="K13" s="8">
         <v>43258.4925</v>
@@ -1726,7 +1727,7 @@
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13905224459</v>
+        <v>15152041534</v>
       </c>
       <c r="K14" s="8">
         <v>43258.522800925923</v>
@@ -1783,7 +1784,7 @@
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13905220263</v>
+        <v>13905221183</v>
       </c>
       <c r="K15" s="8">
         <v>43258.699247685188</v>
@@ -1840,7 +1841,7 @@
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895257241</v>
+        <v>15895252063</v>
       </c>
       <c r="K16" s="8">
         <v>43258.702893518515</v>
@@ -1897,7 +1898,7 @@
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895250087</v>
+        <v>15152043475</v>
       </c>
       <c r="K17" s="8">
         <v>43259.84302083333</v>
@@ -1954,7 +1955,7 @@
       </c>
       <c r="J18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>13905223030</v>
+        <v>13905221479</v>
       </c>
       <c r="K18" s="8">
         <v>43260.833078703705</v>
@@ -2011,7 +2012,7 @@
       </c>
       <c r="J19" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15152041336</v>
+        <v>13905221272</v>
       </c>
       <c r="K19" s="8">
         <v>43261.787499999999</v>
@@ -2068,7 +2069,7 @@
       </c>
       <c r="J20" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15895257991</v>
+        <v>15895258960</v>
       </c>
       <c r="K20" s="8">
         <v>43262.336354166669</v>
@@ -2125,7 +2126,7 @@
       </c>
       <c r="J21" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>15152046250</v>
+        <v>15895259309</v>
       </c>
       <c r="K21" s="8">
         <v>43262.759675925925</v>
@@ -2178,7 +2179,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>

</xml_diff>